<commit_message>
cambio de una linea en python y comienzo de proceso ETL
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_111019.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_111019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3E3F5-922E-47F0-BB38-545F8751D50B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962A3BA4-661E-464E-A01D-0DA552D46A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -1441,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Descarga de todos los csv
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_111019.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_111019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962A3BA4-661E-464E-A01D-0DA552D46A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B422AFD8-0AD9-486E-BEF4-153548E4026D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -915,51 +915,60 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1114,7 +1123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1208,6 +1217,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1443,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -1688,7 +1698,7 @@
       <c r="A18" s="26">
         <v>1.4</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="49" t="s">
         <v>109</v>
       </c>
       <c r="C18" s="28">
@@ -1730,7 +1740,7 @@
       <c r="A21" s="26">
         <v>1.7</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="49" t="s">
         <v>112</v>
       </c>
       <c r="C21" s="28">

</xml_diff>